<commit_message>
Upload file Database, Image login
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lesyt\OneDrive - Thanglele\DATA-LEARNING\C#\SchoolEdu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3F6730F-802B-4DB6-A93B-57AB0D82B5C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20B2B3A-99BB-4FA6-ABBF-BC54C9F42192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7155" yWindow="4065" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{FB706267-7A05-4D03-A38D-A1D6E09A9BBD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{FB706267-7A05-4D03-A38D-A1D6E09A9BBD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Thongtinsinhvien" sheetId="1" r:id="rId1"/>
-    <sheet name="Login_infomation" sheetId="3" r:id="rId2"/>
-    <sheet name="Lichthi" sheetId="2" r:id="rId3"/>
-    <sheet name="Tinchi" sheetId="4" r:id="rId4"/>
-    <sheet name="GPA" sheetId="5" r:id="rId5"/>
-    <sheet name="Trang_tính6" sheetId="6" r:id="rId6"/>
-    <sheet name="Monhoc" sheetId="7" r:id="rId7"/>
+    <sheet name="Tinchi" sheetId="4" r:id="rId1"/>
+    <sheet name="Trang_tính6" sheetId="6" r:id="rId2"/>
+    <sheet name="GIAOVIEN" sheetId="8" r:id="rId3"/>
+    <sheet name="DIEMSV" sheetId="9" r:id="rId4"/>
+    <sheet name="GVMH" sheetId="10" r:id="rId5"/>
+    <sheet name="LOP" sheetId="11" r:id="rId6"/>
+    <sheet name="MONHOC" sheetId="12" r:id="rId7"/>
+    <sheet name="SINHVIEN" sheetId="13" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,13 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="113">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>HoTen</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="137">
   <si>
     <t>NgaySinh</t>
   </si>
@@ -56,48 +51,21 @@
     <t>Khoa</t>
   </si>
   <si>
-    <t>Lop</t>
-  </si>
-  <si>
-    <t>Khoas</t>
-  </si>
-  <si>
     <t>MaTinChi</t>
   </si>
   <si>
-    <t>SoTinChi</t>
-  </si>
-  <si>
     <t>DiemQT</t>
   </si>
   <si>
     <t>DiemThi</t>
   </si>
   <si>
-    <t>GPA</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Mem</t>
-  </si>
-  <si>
-    <t>TenGiaoVien</t>
-  </si>
-  <si>
-    <t>MonThi</t>
-  </si>
-  <si>
     <t>CaThi</t>
   </si>
   <si>
     <t>NgayThi</t>
   </si>
   <si>
-    <t>PhongThi</t>
-  </si>
-  <si>
     <t>TenMonHoc</t>
   </si>
   <si>
@@ -377,20 +345,132 @@
     <t>4.2</t>
   </si>
   <si>
-    <t>Mamonhoc</t>
-  </si>
-  <si>
-    <t>Tenmonhoc</t>
+    <t>MaGV</t>
+  </si>
+  <si>
+    <t>TenGV</t>
+  </si>
+  <si>
+    <t>GioiTinh</t>
+  </si>
+  <si>
+    <t>DiaChi</t>
+  </si>
+  <si>
+    <t>MatKhau</t>
+  </si>
+  <si>
+    <t>VaiTro</t>
+  </si>
+  <si>
+    <t>MaSV</t>
+  </si>
+  <si>
+    <t>MaMH</t>
+  </si>
+  <si>
+    <t>LanThi</t>
+  </si>
+  <si>
+    <t>Ngaybd</t>
+  </si>
+  <si>
+    <t>Phonghoc</t>
+  </si>
+  <si>
+    <t>MaLop</t>
+  </si>
+  <si>
+    <t>Nganh</t>
+  </si>
+  <si>
+    <t>Nienkhoa</t>
+  </si>
+  <si>
+    <t>TenMH</t>
+  </si>
+  <si>
+    <t>SoTC</t>
+  </si>
+  <si>
+    <t>TenSV</t>
+  </si>
+  <si>
+    <t>64ANM1</t>
+  </si>
+  <si>
+    <t>Công nghệ thông tin</t>
+  </si>
+  <si>
+    <t>An ninh mạng</t>
+  </si>
+  <si>
+    <t>K64</t>
+  </si>
+  <si>
+    <t>64ANM2</t>
+  </si>
+  <si>
+    <t>64HTTT1</t>
+  </si>
+  <si>
+    <t>64HTTT2</t>
+  </si>
+  <si>
+    <t>64HTTT3</t>
+  </si>
+  <si>
+    <t>64HTTT4</t>
+  </si>
+  <si>
+    <t>Hệ thống thông tin</t>
+  </si>
+  <si>
+    <t>64CNTT1</t>
+  </si>
+  <si>
+    <t>64CNTT2</t>
+  </si>
+  <si>
+    <t>64TTNT1</t>
+  </si>
+  <si>
+    <t>64TTNT2</t>
+  </si>
+  <si>
+    <t>64KTPM1</t>
+  </si>
+  <si>
+    <t>64KTPM2</t>
+  </si>
+  <si>
+    <t>64KTPM3</t>
+  </si>
+  <si>
+    <t>64KTPM4</t>
+  </si>
+  <si>
+    <t>64KTPM5</t>
+  </si>
+  <si>
+    <t>Kỹ thuật phần mềm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
@@ -552,8 +632,8 @@
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>257175</xdr:colOff>
-          <xdr:row>0</xdr:row>
-          <xdr:rowOff>257175</xdr:rowOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -563,7 +643,7 @@
                   <a14:compatExt spid="_x0000_s6145"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09B0B634-D548-D56E-20C7-A7DE139B2841}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000001180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -613,7 +693,7 @@
                   <a14:compatExt spid="_x0000_s6146"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60B389DE-8CF4-2DE4-CA68-0B06F35BC5A8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -652,8 +732,8 @@
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>257175</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>257175</xdr:rowOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -663,7 +743,7 @@
                   <a14:compatExt spid="_x0000_s6147"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F6C59FA-CCBB-FB67-8D0E-88577EBF1644}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -702,8 +782,8 @@
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>257175</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>257175</xdr:rowOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -713,7 +793,7 @@
                   <a14:compatExt spid="_x0000_s6148"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C4E28F1-6E7F-D393-3627-13496E6E20A7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -752,8 +832,8 @@
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>257175</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>257175</xdr:rowOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -763,7 +843,7 @@
                   <a14:compatExt spid="_x0000_s6149"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C5DA9E5-2008-D96F-D7BC-8D5B600F50F0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -813,7 +893,7 @@
                   <a14:compatExt spid="_x0000_s6150"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3444187-93E2-156C-B70B-789153E75E3B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -852,8 +932,8 @@
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>257175</xdr:colOff>
-          <xdr:row>6</xdr:row>
-          <xdr:rowOff>257175</xdr:rowOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -863,7 +943,7 @@
                   <a14:compatExt spid="_x0000_s6151"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C098A92E-B208-2ADD-9C82-90FE16DAE75A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -902,8 +982,8 @@
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>257175</xdr:colOff>
-          <xdr:row>7</xdr:row>
-          <xdr:rowOff>257175</xdr:rowOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -913,7 +993,7 @@
                   <a14:compatExt spid="_x0000_s6152"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2FD5909-189A-583D-B123-040D35CDD365}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000008180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -952,8 +1032,8 @@
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>257175</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>257175</xdr:rowOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -963,7 +1043,7 @@
                   <a14:compatExt spid="_x0000_s6153"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7511B315-CE3E-65B2-DA03-676B2997CC7B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1013,7 +1093,7 @@
                   <a14:compatExt spid="_x0000_s6154"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A2E3F4E-26A5-73AE-C3DC-57472EF35E59}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000A180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1063,7 +1143,7 @@
                   <a14:compatExt spid="_x0000_s6155"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71DA8DFD-6F72-3D8C-7444-2872C06C1C10}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000B180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1102,8 +1182,8 @@
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>257175</xdr:colOff>
-          <xdr:row>11</xdr:row>
-          <xdr:rowOff>257175</xdr:rowOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1113,7 +1193,7 @@
                   <a14:compatExt spid="_x0000_s6156"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C6030C5-E4CC-07BA-7733-0C6B40B7DA14}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000C180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1152,8 +1232,8 @@
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>257175</xdr:colOff>
-          <xdr:row>12</xdr:row>
-          <xdr:rowOff>257175</xdr:rowOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1163,7 +1243,7 @@
                   <a14:compatExt spid="_x0000_s6157"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38D7F9CB-F5A7-F69C-497C-C1CEF899102E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000D180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1213,7 +1293,7 @@
                   <a14:compatExt spid="_x0000_s6158"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EBB4271-2DDF-5F4E-6F01-86C73A063136}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000E180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1252,8 +1332,8 @@
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>257175</xdr:colOff>
-          <xdr:row>14</xdr:row>
-          <xdr:rowOff>257175</xdr:rowOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1263,7 +1343,7 @@
                   <a14:compatExt spid="_x0000_s6159"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BEE7C03F-F355-0F09-2C68-B7BB9509D238}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000F180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1313,7 +1393,7 @@
                   <a14:compatExt spid="_x0000_s6160"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{983C33F2-3B71-6E6C-2A65-A4DFB30982C0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000010180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1352,8 +1432,8 @@
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>257175</xdr:colOff>
-          <xdr:row>16</xdr:row>
-          <xdr:rowOff>257175</xdr:rowOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1363,7 +1443,7 @@
                   <a14:compatExt spid="_x0000_s6161"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02364CEB-B3D1-FD05-139D-B440F1C6ABD7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000011180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1413,7 +1493,7 @@
                   <a14:compatExt spid="_x0000_s6162"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D0C67F8-4A7C-6692-AFE9-2D1CC69EC2B8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000012180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1452,8 +1532,8 @@
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>257175</xdr:colOff>
-          <xdr:row>18</xdr:row>
-          <xdr:rowOff>257175</xdr:rowOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1463,7 +1543,7 @@
                   <a14:compatExt spid="_x0000_s6163"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6A8ADB9-2091-41FB-9608-3D84FD4AE016}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000013180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1502,8 +1582,8 @@
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>257175</xdr:colOff>
-          <xdr:row>19</xdr:row>
-          <xdr:rowOff>257175</xdr:rowOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1513,7 +1593,7 @@
                   <a14:compatExt spid="_x0000_s6164"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3DC659F-A80E-31CD-A23A-3E4777A64D83}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000014180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1552,8 +1632,8 @@
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>257175</xdr:colOff>
-          <xdr:row>20</xdr:row>
-          <xdr:rowOff>257175</xdr:rowOff>
+          <xdr:row>21</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1563,7 +1643,7 @@
                   <a14:compatExt spid="_x0000_s6165"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A75D957-845E-FFCD-A97F-162232F9B1FE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000015180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1602,8 +1682,8 @@
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>257175</xdr:colOff>
-          <xdr:row>21</xdr:row>
-          <xdr:rowOff>257175</xdr:rowOff>
+          <xdr:row>22</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1613,7 +1693,7 @@
                   <a14:compatExt spid="_x0000_s6166"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F65312B-E4CD-6EB7-363A-1A02C433D35F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000016180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1663,7 +1743,7 @@
                   <a14:compatExt spid="_x0000_s6167"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{525A8239-4DC6-ADF9-8DB7-E6B4D27F9523}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000017180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1702,8 +1782,8 @@
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>257175</xdr:colOff>
-          <xdr:row>23</xdr:row>
-          <xdr:rowOff>257175</xdr:rowOff>
+          <xdr:row>24</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1713,7 +1793,7 @@
                   <a14:compatExt spid="_x0000_s6168"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F204D17E-0688-F395-46A2-F25F18CB57F4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000018180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2059,118 +2139,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BEDA8B-C007-476C-B301-BA9C4A0F6874}">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.375" customWidth="1"/>
-    <col min="2" max="2" width="18.125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95BB98F-9E06-4871-82E1-4E86F24A6E77}">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="18.125" customWidth="1"/>
-    <col min="3" max="3" width="17.875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D45ABD24-E867-464B-A247-F007B4126524}">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="16.25" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA5AFDA-7738-41DF-B305-53CBCC31CC6E}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2186,217 +2159,217 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="2" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="B11" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2404,47 +2377,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4AEB537-0E19-4889-AA33-2BD3648F023B}">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982953CC-907D-497F-96C1-26A39BB8805C}">
   <sheetPr codeName="Trang_tính1"/>
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
@@ -2455,15 +2393,15 @@
     <col min="9" max="9" width="18.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1">
         <v>1</v>
@@ -2476,7 +2414,7 @@
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I1" s="1">
         <v>2251172491</v>
@@ -2491,7 +2429,7 @@
         <v>5</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
@@ -2499,10 +2437,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -2515,7 +2453,7 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="I2" s="1">
         <v>2251172491</v>
@@ -2530,18 +2468,18 @@
         <v>0</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="57" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1">
         <v>3</v>
@@ -2554,33 +2492,33 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I3" s="1">
         <v>2251172491</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="L3" s="1">
         <v>8</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1">
         <v>3</v>
@@ -2593,33 +2531,33 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I4" s="1">
         <v>2251172491</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1">
         <v>3</v>
@@ -2632,22 +2570,22 @@
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I5" s="1">
         <v>2251172491</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -2655,10 +2593,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -2671,7 +2609,7 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I6" s="1">
         <v>2251172491</v>
@@ -2683,21 +2621,21 @@
         <v>6</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D7" s="1">
         <v>3</v>
@@ -2710,33 +2648,33 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I7" s="1">
         <v>2251172491</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="57" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="D8" s="1">
         <v>3</v>
@@ -2749,7 +2687,7 @@
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I8" s="1">
         <v>2251172491</v>
@@ -2761,21 +2699,21 @@
         <v>5</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="D9" s="1">
         <v>3</v>
@@ -2788,7 +2726,7 @@
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I9" s="1">
         <v>2251172491</v>
@@ -2797,24 +2735,24 @@
         <v>8</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="D10" s="1">
         <v>3</v>
@@ -2827,7 +2765,7 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I10" s="1">
         <v>2251172491</v>
@@ -2839,21 +2777,21 @@
         <v>7</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D11" s="1">
         <v>2</v>
@@ -2866,33 +2804,33 @@
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I11" s="1">
         <v>2251172491</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="K11" s="1">
         <v>7</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D12" s="1">
         <v>3</v>
@@ -2905,33 +2843,33 @@
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I12" s="1">
         <v>2251172491</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D13" s="1">
         <v>3</v>
@@ -2944,7 +2882,7 @@
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I13" s="1">
         <v>2251172491</v>
@@ -2953,24 +2891,24 @@
         <v>10</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="57" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="D14" s="1">
         <v>3</v>
@@ -2983,33 +2921,33 @@
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I14" s="1">
         <v>2251172491</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D15" s="1">
         <v>3</v>
@@ -3022,22 +2960,22 @@
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I15" s="1">
         <v>2251172491</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -3045,10 +2983,10 @@
         <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
@@ -3061,7 +2999,7 @@
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I16" s="1">
         <v>2251172491</v>
@@ -3076,18 +3014,18 @@
         <v>9</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="D17" s="1">
         <v>3</v>
@@ -3100,22 +3038,22 @@
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I17" s="1">
         <v>2251172491</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
@@ -3123,10 +3061,10 @@
         <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="D18" s="1">
         <v>3</v>
@@ -3139,33 +3077,33 @@
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="I18" s="1">
         <v>2251172491</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="K18" s="1">
         <v>0</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="D19" s="1">
         <v>6</v>
@@ -3178,7 +3116,7 @@
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I19" s="1">
         <v>2251172491</v>
@@ -3186,21 +3124,21 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D20" s="1">
         <v>3</v>
@@ -3213,33 +3151,33 @@
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I20" s="1">
         <v>2251172491</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="D21" s="1">
         <v>3</v>
@@ -3252,33 +3190,33 @@
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I21" s="1">
         <v>2251172491</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="D22" s="1">
         <v>3</v>
@@ -3291,22 +3229,22 @@
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I22" s="1">
         <v>2251172491</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="K22" s="1">
         <v>8</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -3314,10 +3252,10 @@
         <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
@@ -3330,7 +3268,7 @@
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I23" s="1">
         <v>2251172491</v>
@@ -3342,21 +3280,21 @@
         <v>7</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="D24" s="1">
         <v>3</v>
@@ -3369,22 +3307,22 @@
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I24" s="1">
         <v>2251172491</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="K24" s="1">
         <v>2</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -3394,19 +3332,44 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="6168" r:id="rId3" name="Control 24">
+        <control shapeId="6145" r:id="rId3" name="Control 1">
           <controlPr defaultSize="0" r:id="rId4">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>23</xdr:row>
+                <xdr:row>0</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>23</xdr:row>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="6145" r:id="rId3" name="Control 1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="6146" r:id="rId5" name="Control 2">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>1</xdr:row>
                 <xdr:rowOff>257175</xdr:rowOff>
               </to>
             </anchor>
@@ -3414,13 +3377,513 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="6168" r:id="rId3" name="Control 24"/>
+        <control shapeId="6146" r:id="rId5" name="Control 2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="6167" r:id="rId5" name="Control 23">
-          <controlPr defaultSize="0" r:id="rId6">
+        <control shapeId="6147" r:id="rId6" name="Control 3">
+          <controlPr defaultSize="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="6147" r:id="rId6" name="Control 3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="6148" r:id="rId8" name="Control 4">
+          <controlPr defaultSize="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="6148" r:id="rId8" name="Control 4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="6149" r:id="rId9" name="Control 5">
+          <controlPr defaultSize="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="6149" r:id="rId9" name="Control 5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="6150" r:id="rId10" name="Control 6">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="6150" r:id="rId10" name="Control 6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="6151" r:id="rId11" name="Control 7">
+          <controlPr defaultSize="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="6151" r:id="rId11" name="Control 7"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="6152" r:id="rId12" name="Control 8">
+          <controlPr defaultSize="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="6152" r:id="rId12" name="Control 8"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="6153" r:id="rId13" name="Control 9">
+          <controlPr defaultSize="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="6153" r:id="rId13" name="Control 9"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="6154" r:id="rId14" name="Control 10">
+          <controlPr defaultSize="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>257175</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="6154" r:id="rId14" name="Control 10"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="6155" r:id="rId15" name="Control 11">
+          <controlPr defaultSize="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>257175</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="6155" r:id="rId15" name="Control 11"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="6156" r:id="rId16" name="Control 12">
+          <controlPr defaultSize="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="6156" r:id="rId16" name="Control 12"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="6157" r:id="rId17" name="Control 13">
+          <controlPr defaultSize="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="6157" r:id="rId17" name="Control 13"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="6158" r:id="rId18" name="Control 14">
+          <controlPr defaultSize="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>257175</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="6158" r:id="rId18" name="Control 14"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="6159" r:id="rId19" name="Control 15">
+          <controlPr defaultSize="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="6159" r:id="rId19" name="Control 15"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="6160" r:id="rId20" name="Control 16">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="6160" r:id="rId20" name="Control 16"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="6161" r:id="rId21" name="Control 17">
+          <controlPr defaultSize="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="6161" r:id="rId21" name="Control 17"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="6162" r:id="rId22" name="Control 18">
+          <controlPr defaultSize="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>257175</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="6162" r:id="rId22" name="Control 18"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="6163" r:id="rId23" name="Control 19">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>19</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="6163" r:id="rId23" name="Control 19"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="6164" r:id="rId24" name="Control 20">
+          <controlPr defaultSize="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>19</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="6164" r:id="rId24" name="Control 20"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="6165" r:id="rId25" name="Control 21">
+          <controlPr defaultSize="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="6165" r:id="rId25" name="Control 21"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="6166" r:id="rId26" name="Control 22">
+          <controlPr defaultSize="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>22</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="6166" r:id="rId26" name="Control 22"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="6167" r:id="rId27" name="Control 23">
+          <controlPr defaultSize="0" r:id="rId4">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
@@ -3439,174 +3902,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="6167" r:id="rId5" name="Control 23"/>
+        <control shapeId="6167" r:id="rId27" name="Control 23"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="6166" r:id="rId7" name="Control 22">
-          <controlPr defaultSize="0" r:id="rId4">
+        <control shapeId="6168" r:id="rId28" name="Control 24">
+          <controlPr defaultSize="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>21</xdr:row>
+                <xdr:row>23</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>257175</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="6166" r:id="rId7" name="Control 22"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="6165" r:id="rId8" name="Control 21">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>257175</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="6165" r:id="rId8" name="Control 21"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="6164" r:id="rId9" name="Control 20">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>19</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>19</xdr:row>
-                <xdr:rowOff>257175</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="6164" r:id="rId9" name="Control 20"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="6163" r:id="rId10" name="Control 19">
-          <controlPr defaultSize="0" r:id="rId6">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>257175</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="6163" r:id="rId10" name="Control 19"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="6162" r:id="rId11" name="Control 18">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>257175</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="6162" r:id="rId11" name="Control 18"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="6161" r:id="rId12" name="Control 17">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>257175</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="6161" r:id="rId12" name="Control 17"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="6160" r:id="rId13" name="Control 16">
-          <controlPr defaultSize="0" r:id="rId6">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>15</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>16</xdr:row>
+                <xdr:row>24</xdr:row>
                 <xdr:rowOff>76200</xdr:rowOff>
               </to>
             </anchor>
@@ -3614,408 +3927,698 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="6160" r:id="rId13" name="Control 16"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="6159" r:id="rId14" name="Control 15">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>257175</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="6159" r:id="rId14" name="Control 15"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="6158" r:id="rId15" name="Control 14">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>257175</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="6158" r:id="rId15" name="Control 14"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="6157" r:id="rId16" name="Control 13">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>257175</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="6157" r:id="rId16" name="Control 13"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="6156" r:id="rId17" name="Control 12">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>257175</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="6156" r:id="rId17" name="Control 12"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="6155" r:id="rId18" name="Control 11">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>257175</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="6155" r:id="rId18" name="Control 11"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="6154" r:id="rId19" name="Control 10">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>257175</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="6154" r:id="rId19" name="Control 10"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="6153" r:id="rId20" name="Control 9">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>257175</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="6153" r:id="rId20" name="Control 9"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="6152" r:id="rId21" name="Control 8">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>257175</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="6152" r:id="rId21" name="Control 8"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="6151" r:id="rId22" name="Control 7">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>257175</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="6151" r:id="rId22" name="Control 7"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="6150" r:id="rId23" name="Control 6">
-          <controlPr defaultSize="0" r:id="rId6">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="6150" r:id="rId23" name="Control 6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="6149" r:id="rId24" name="Control 5">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>257175</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="6149" r:id="rId24" name="Control 5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="6148" r:id="rId25" name="Control 4">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>257175</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="6148" r:id="rId25" name="Control 4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="6147" r:id="rId26" name="Control 3">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>257175</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="6147" r:id="rId26" name="Control 3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="6146" r:id="rId27" name="Control 2">
-          <controlPr defaultSize="0" r:id="rId6">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>257175</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="6146" r:id="rId27" name="Control 2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="6145" r:id="rId28" name="Control 1">
-          <controlPr defaultSize="0" r:id="rId6">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>257175</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="6145" r:id="rId28" name="Control 1"/>
+        <control shapeId="6168" r:id="rId28" name="Control 24"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{449C5CD5-C880-4898-ACB1-315D3BB461B0}">
-  <dimension ref="A1:B1"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB644288-C5A7-4418-B163-6911149B6A64}">
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{551ACEE3-73EF-4115-BBA9-F8FA495F16EC}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB6EF398-9BFC-43CC-A7CB-A4F83E819CCE}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.625" customWidth="1"/>
+    <col min="3" max="3" width="12.125" customWidth="1"/>
+    <col min="4" max="4" width="11.125" customWidth="1"/>
+    <col min="5" max="5" width="11.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3865EC66-606D-49A9-8C94-908A6D1C15A6}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.625" customWidth="1"/>
+    <col min="2" max="3" width="17.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>111</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>112</v>
+      </c>
+      <c r="D1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" t="s">
+        <v>136</v>
+      </c>
+      <c r="D12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" t="s">
+        <v>136</v>
+      </c>
+      <c r="D13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" t="s">
+        <v>136</v>
+      </c>
+      <c r="D14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" t="s">
+        <v>136</v>
+      </c>
+      <c r="D15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" t="s">
+        <v>136</v>
+      </c>
+      <c r="D16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057CD0B1-CE2C-42F9-84CC-2B1BEA1CD256}">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="32.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{250D15DE-FAC0-4023-8A0F-5ADAD22EF218}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>